<commit_message>
Aggiunta terza tabella temporanea indicatori retail
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17870"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="Fields definition" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variable!$A$2:$M$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variable!$A$1:$N$86</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -469,63 +469,6 @@
     <t>IsCustomField</t>
   </si>
   <si>
-    <t xml:space="preserve">RETAIL_IND_52 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_53 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_54 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_55 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_60 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_61 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_62 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_63 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_64 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_70 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_71 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_80 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_81 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_82 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_83 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_84 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_85 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_86 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RETAIL_IND_87 </t>
-  </si>
-  <si>
     <t>RETAIL_IND_100</t>
   </si>
   <si>
@@ -623,63 +566,6 @@
   </si>
   <si>
     <t>RETAIL_IND_231</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_52 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_53 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_54 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_55 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_60 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_61 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_62 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_63 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_64 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_70 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_71 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_80 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_81 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_82 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_83 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_84 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_85 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_86 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IND_87 </t>
   </si>
   <si>
     <t>IND_100</t>
@@ -1223,11 +1109,125 @@
 - "1" in assenza di uno sconfino nell'ultimo mese e in presenza di uno sconfino fra i 60 e i 30 giorni antecedenti la data di elaborazione; 
 </t>
   </si>
+  <si>
+    <t>RETAIL_IND_52</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_53</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_54</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_55</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_60</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_61</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_62</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_63</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_64</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_70</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_71</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_80</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_81</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_82</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_83</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_84</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_85</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_86</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_87</t>
+  </si>
+  <si>
+    <t>IND_52</t>
+  </si>
+  <si>
+    <t>IND_53</t>
+  </si>
+  <si>
+    <t>IND_54</t>
+  </si>
+  <si>
+    <t>IND_55</t>
+  </si>
+  <si>
+    <t>IND_60</t>
+  </si>
+  <si>
+    <t>IND_61</t>
+  </si>
+  <si>
+    <t>IND_62</t>
+  </si>
+  <si>
+    <t>IND_63</t>
+  </si>
+  <si>
+    <t>IND_64</t>
+  </si>
+  <si>
+    <t>IND_70</t>
+  </si>
+  <si>
+    <t>IND_71</t>
+  </si>
+  <si>
+    <t>IND_80</t>
+  </si>
+  <si>
+    <t>IND_81</t>
+  </si>
+  <si>
+    <t>IND_82</t>
+  </si>
+  <si>
+    <t>IND_83</t>
+  </si>
+  <si>
+    <t>IND_84</t>
+  </si>
+  <si>
+    <t>IND_85</t>
+  </si>
+  <si>
+    <t>IND_86</t>
+  </si>
+  <si>
+    <t>IND_87</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1565,7 +1565,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1623,7 +1629,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1681,7 +1693,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1739,7 +1757,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1797,7 +1821,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1855,7 +1885,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1903,7 +1939,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvPr id="13" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1961,7 +2003,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvPr id="14" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2019,7 +2067,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvPr id="15" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2077,7 +2131,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvPr id="16" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2135,7 +2195,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="CustomShape 1"/>
+        <xdr:cNvPr id="17" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2193,7 +2259,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3074" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="3074" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000020C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -2489,30 +2561,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L81" sqref="L81"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.83984375" style="15" customWidth="1"/>
     <col min="2" max="2" width="21" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66.68359375" customWidth="1"/>
+    <col min="5" max="5" width="22.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.578125" customWidth="1"/>
     <col min="7" max="7" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="1021" width="8.7109375"/>
+    <col min="8" max="8" width="21.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.41796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.68359375" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.15625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.26171875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.15625" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="1019" width="8.68359375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2530,7 +2602,7 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
@@ -2574,7 +2646,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="22" t="s">
         <v>11</v>
       </c>
@@ -2618,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
@@ -2706,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -2750,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -2794,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
@@ -2838,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
@@ -2882,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="20" t="s">
         <v>11</v>
       </c>
@@ -2926,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
@@ -2970,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
@@ -3014,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -3058,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="20" t="s">
         <v>11</v>
       </c>
@@ -3102,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
@@ -3146,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="20" t="s">
         <v>11</v>
       </c>
@@ -3190,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="20" t="s">
         <v>11</v>
       </c>
@@ -3234,7 +3306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="20" t="s">
         <v>11</v>
       </c>
@@ -3278,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="20" t="s">
         <v>11</v>
       </c>
@@ -3322,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="20" t="s">
         <v>11</v>
       </c>
@@ -3366,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="20" t="s">
         <v>11</v>
       </c>
@@ -3410,7 +3482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
@@ -3454,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="20" t="s">
         <v>11</v>
       </c>
@@ -3498,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
@@ -3542,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="20" t="s">
         <v>11</v>
       </c>
@@ -3586,24 +3658,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="E26" t="s">
-        <v>190</v>
+        <v>363</v>
       </c>
       <c r="F26" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="G26" s="14">
         <v>223</v>
@@ -3630,24 +3702,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
       <c r="D27" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>364</v>
       </c>
       <c r="F27" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="G27" s="14">
         <v>224</v>
@@ -3674,24 +3746,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
       <c r="E28" t="s">
-        <v>192</v>
+        <v>365</v>
       </c>
       <c r="F28" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
       <c r="G28" s="14">
         <v>225</v>
@@ -3718,24 +3790,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E29" t="s">
-        <v>193</v>
+        <v>366</v>
       </c>
       <c r="F29" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="G29" s="14">
         <v>226</v>
@@ -3762,24 +3834,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="D30" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>367</v>
       </c>
       <c r="F30" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="G30" s="14">
         <v>227</v>
@@ -3806,24 +3878,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>143</v>
+        <v>349</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>349</v>
       </c>
       <c r="D31" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="E31" t="s">
-        <v>195</v>
+        <v>368</v>
       </c>
       <c r="F31" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="G31" s="14">
         <v>228</v>
@@ -3850,24 +3922,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="D32" t="s">
-        <v>246</v>
+        <v>208</v>
       </c>
       <c r="E32" t="s">
-        <v>196</v>
+        <v>369</v>
       </c>
       <c r="F32" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="G32" s="14">
         <v>229</v>
@@ -3894,24 +3966,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="D33" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="E33" t="s">
-        <v>197</v>
+        <v>370</v>
       </c>
       <c r="F33" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="G33" s="14">
         <v>230</v>
@@ -3938,24 +4010,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="D34" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>371</v>
       </c>
       <c r="F34" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="G34" s="14">
         <v>231</v>
@@ -3982,24 +4054,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="D35" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="E35" t="s">
-        <v>199</v>
+        <v>372</v>
       </c>
       <c r="F35" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="G35" s="14">
         <v>232</v>
@@ -4026,24 +4098,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>148</v>
+        <v>354</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>354</v>
       </c>
       <c r="D36" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="E36" t="s">
-        <v>200</v>
+        <v>373</v>
       </c>
       <c r="F36" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="G36" s="14">
         <v>233</v>
@@ -4070,24 +4142,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
       <c r="D37" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="E37" t="s">
-        <v>201</v>
+        <v>374</v>
       </c>
       <c r="F37" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="G37" s="14">
         <v>234</v>
@@ -4114,24 +4186,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="D38" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="E38" t="s">
-        <v>202</v>
+        <v>375</v>
       </c>
       <c r="F38" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="G38" s="14">
         <v>235</v>
@@ -4158,24 +4230,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>151</v>
+        <v>357</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>357</v>
       </c>
       <c r="D39" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="E39" t="s">
-        <v>203</v>
+        <v>376</v>
       </c>
       <c r="F39" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="G39" s="14">
         <v>236</v>
@@ -4202,24 +4274,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="D40" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="E40" t="s">
-        <v>204</v>
+        <v>377</v>
       </c>
       <c r="F40" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="G40" s="14">
         <v>237</v>
@@ -4246,24 +4318,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>153</v>
+        <v>359</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>359</v>
       </c>
       <c r="D41" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="E41" t="s">
-        <v>205</v>
+        <v>378</v>
       </c>
       <c r="F41" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="G41" s="14">
         <v>238</v>
@@ -4290,24 +4362,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>154</v>
+        <v>360</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>360</v>
       </c>
       <c r="D42" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="E42" t="s">
-        <v>206</v>
+        <v>379</v>
       </c>
       <c r="F42" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="G42" s="14">
         <v>239</v>
@@ -4334,24 +4406,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="D43" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="E43" t="s">
-        <v>207</v>
+        <v>380</v>
       </c>
       <c r="F43" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="G43" s="14">
         <v>240</v>
@@ -4378,24 +4450,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
       <c r="E44" t="s">
-        <v>208</v>
+        <v>381</v>
       </c>
       <c r="F44" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G44" s="14">
         <v>241</v>
@@ -4422,24 +4494,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
       <c r="E45" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="F45" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="G45" s="14">
         <v>242</v>
@@ -4466,24 +4538,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="D46" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="E46" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="F46" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="G46" s="14">
         <v>243</v>
@@ -4510,24 +4582,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="E47" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="F47" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="G47" s="14">
         <v>244</v>
@@ -4554,24 +4626,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
       <c r="E48" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="F48" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="G48" s="14">
         <v>245</v>
@@ -4598,24 +4670,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D49" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
       <c r="E49" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="F49" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="G49" s="14">
         <v>246</v>
@@ -4642,24 +4714,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D50" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
       <c r="E50" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="F50" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="G50" s="14">
         <v>247</v>
@@ -4686,24 +4758,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="D51" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
       <c r="E51" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="F51" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="G51" s="14">
         <v>248</v>
@@ -4730,24 +4802,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="D52" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
       <c r="E52" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="F52" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="G52" s="14">
         <v>249</v>
@@ -4774,24 +4846,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D53" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
       <c r="E53" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="F53" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="G53" s="14">
         <v>250</v>
@@ -4818,24 +4890,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D54" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
       <c r="E54" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="F54" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="G54" s="14">
         <v>251</v>
@@ -4862,24 +4934,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
       <c r="E55" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
       <c r="F55" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="G55" s="14">
         <v>252</v>
@@ -4906,24 +4978,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="E56" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="F56" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="G56" s="14">
         <v>253</v>
@@ -4950,24 +5022,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="D57" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
       <c r="E57" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="F57" t="s">
-        <v>291</v>
+        <v>253</v>
       </c>
       <c r="G57" s="14">
         <v>254</v>
@@ -4994,24 +5066,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="D58" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
       <c r="E58" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="F58" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="G58" s="14">
         <v>255</v>
@@ -5038,24 +5110,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D59" t="s">
-        <v>324</v>
+        <v>286</v>
       </c>
       <c r="E59" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="F59" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="G59" s="14">
         <v>256</v>
@@ -5082,24 +5154,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D60" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="E60" t="s">
-        <v>224</v>
+        <v>186</v>
       </c>
       <c r="F60" t="s">
-        <v>294</v>
+        <v>256</v>
       </c>
       <c r="G60" s="14">
         <v>257</v>
@@ -5126,24 +5198,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D61" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
       <c r="E61" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="F61" t="s">
-        <v>295</v>
+        <v>257</v>
       </c>
       <c r="G61" s="14">
         <v>258</v>
@@ -5170,24 +5242,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D62" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
       <c r="E62" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="F62" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
       <c r="G62" s="14">
         <v>259</v>
@@ -5214,24 +5286,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="E63" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="F63" t="s">
-        <v>297</v>
+        <v>259</v>
       </c>
       <c r="G63" s="14">
         <v>260</v>
@@ -5258,24 +5330,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
       <c r="E64" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="F64" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="G64" s="14">
         <v>261</v>
@@ -5302,24 +5374,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="D65" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
       <c r="E65" t="s">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="F65" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="G65" s="14">
         <v>262</v>
@@ -5346,24 +5418,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="D66" t="s">
-        <v>331</v>
+        <v>293</v>
       </c>
       <c r="E66" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="F66" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="G66" s="14">
         <v>263</v>
@@ -5390,24 +5462,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="D67" t="s">
-        <v>332</v>
+        <v>294</v>
       </c>
       <c r="E67" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="F67" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="G67" s="14">
         <v>264</v>
@@ -5434,24 +5506,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="D68" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="F68" t="s">
-        <v>302</v>
+        <v>264</v>
       </c>
       <c r="G68" s="14">
         <v>265</v>
@@ -5478,24 +5550,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="C69" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="D69" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
       <c r="E69" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="F69" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="G69" s="14">
         <v>266</v>
@@ -5522,24 +5594,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="D70" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
       <c r="E70" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="F70" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="G70" s="14">
         <v>267</v>
@@ -5566,24 +5638,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D71" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
       <c r="E71" t="s">
-        <v>235</v>
+        <v>197</v>
       </c>
       <c r="F71" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="G71" s="14">
         <v>268</v>
@@ -5610,24 +5682,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="D72" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
       <c r="E72" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="F72" t="s">
-        <v>306</v>
+        <v>268</v>
       </c>
       <c r="G72" s="14">
         <v>269</v>
@@ -5654,24 +5726,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="D73" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
       <c r="E73" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="F73" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="G73" s="14">
         <v>270</v>
@@ -5698,24 +5770,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="D74" t="s">
-        <v>339</v>
+        <v>301</v>
       </c>
       <c r="E74" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
       <c r="F74" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
       <c r="G74" s="14">
         <v>271</v>
@@ -5742,24 +5814,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D75" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
       <c r="E75" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="F75" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="G75" s="14">
         <v>272</v>
@@ -5786,24 +5858,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D76" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
       <c r="E76" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="F76" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
       <c r="G76" s="14">
         <v>273</v>
@@ -5830,24 +5902,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="D77" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
       <c r="E77" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="F77" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="G77" s="14">
         <v>274</v>
@@ -5874,24 +5946,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="C78" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="D78" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
       <c r="E78" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
       <c r="F78" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="G78" s="14">
         <v>275</v>
@@ -5918,24 +5990,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="C79" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="D79" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
       <c r="E79" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
       <c r="F79" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
       <c r="G79" s="14">
         <v>276</v>
@@ -5962,24 +6034,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="C80" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="D80" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
       <c r="E80" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
       <c r="F80" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
       <c r="G80" s="14">
         <v>277</v>
@@ -6006,24 +6078,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="C81" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="D81" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
       <c r="E81" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
       <c r="F81" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
       <c r="G81" s="14">
         <v>278</v>
@@ -6050,24 +6122,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="C82" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="D82" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
       <c r="E82" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
       <c r="F82" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
       <c r="G82" s="14">
         <v>279</v>
@@ -6094,24 +6166,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="C83" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="D83" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="E83" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
       <c r="F83" t="s">
-        <v>366</v>
+        <v>328</v>
       </c>
       <c r="G83" s="14">
         <v>280</v>
@@ -6138,24 +6210,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="C84" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="D84" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="E84" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="F84" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
       <c r="G84" s="14">
         <v>283</v>
@@ -6182,24 +6254,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="C85" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
       <c r="E85" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="F85" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
       <c r="G85" s="14">
         <v>284</v>
@@ -6226,24 +6298,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="C86" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
       <c r="E86" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="F86" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
       <c r="G86" s="14">
         <v>285</v>
@@ -6271,7 +6343,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6282,22 +6353,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A84:XFD85"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.15625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375"/>
+    <col min="5" max="5" width="40.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="1025" width="8.68359375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -6307,7 +6378,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="27"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6327,7 +6398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -6344,7 +6415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -6361,7 +6432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -6378,7 +6449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6395,7 +6466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -6412,7 +6483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6429,7 +6500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -6446,7 +6517,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6463,7 +6534,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -6480,7 +6551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6497,7 +6568,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -6514,7 +6585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -6531,7 +6602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -6548,7 +6619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -6565,7 +6636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -6582,7 +6653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -6599,7 +6670,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -6616,7 +6687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -6633,7 +6704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -6650,7 +6721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -6667,7 +6738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -6684,7 +6755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -6701,7 +6772,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -6718,1038 +6789,1038 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>344</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
       <c r="C27" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="F28" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>349</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>349</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>349</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>350</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>352</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="E35" t="s">
-        <v>147</v>
+        <v>353</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>354</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>354</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>354</v>
       </c>
       <c r="F36" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>355</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="E38" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>357</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
+        <v>357</v>
       </c>
       <c r="E39" t="s">
-        <v>151</v>
+        <v>357</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>358</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>359</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>359</v>
       </c>
       <c r="E41" t="s">
-        <v>153</v>
+        <v>359</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>154</v>
+        <v>360</v>
       </c>
       <c r="C42" t="s">
-        <v>154</v>
+        <v>360</v>
       </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>360</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="E43" t="s">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>362</v>
       </c>
       <c r="F44" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="F45" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E48" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="F48" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="E49" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="F49" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E51" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="F51" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="E52" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="E53" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="E54" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="E56" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="F56" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E57" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="F57" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="F58" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="E59" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="F59" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="F60" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>11</v>
       </c>
       <c r="B61" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E61" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="F61" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>11</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="E64" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F64" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>11</v>
       </c>
       <c r="B65" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="E65" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="E66" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="F66" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="E67" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="F67" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E68" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="F68" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="C69" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="E69" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="F69" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>11</v>
       </c>
       <c r="B70" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="E70" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="F70" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="E71" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="F71" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>11</v>
       </c>
       <c r="B72" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E72" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="F72" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>11</v>
       </c>
       <c r="B73" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="E73" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F73" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>11</v>
       </c>
       <c r="B74" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="E74" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="F74" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="C75" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="E75" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="F75" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>11</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="E76" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F76" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="E77" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F77" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>11</v>
       </c>
       <c r="B78" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="C78" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="E78" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
       <c r="F78" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="C79" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="E79" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
       <c r="F79" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>11</v>
       </c>
       <c r="B80" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="C80" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="E80" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
       <c r="F80" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>11</v>
       </c>
       <c r="B81" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="C81" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="E81" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
       <c r="F81" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>11</v>
       </c>
       <c r="B82" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="C82" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="E82" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="F82" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="C83" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="E83" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="F83" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="C84" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="E84" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
       <c r="F84" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="C85" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="E85" t="s">
-        <v>350</v>
+        <v>312</v>
       </c>
       <c r="F85" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="C86" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="E86" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
       <c r="F86" s="17" t="s">
         <v>22</v>
@@ -7771,19 +7842,19 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="27.28515625"/>
-    <col min="2" max="3" width="19.5703125"/>
-    <col min="4" max="4" width="13.7109375"/>
-    <col min="5" max="7" width="11.7109375"/>
-    <col min="8" max="8" width="19.5703125"/>
+    <col min="1" max="1" width="27.26171875"/>
+    <col min="2" max="3" width="19.578125"/>
+    <col min="4" max="4" width="13.68359375"/>
+    <col min="5" max="7" width="11.68359375"/>
+    <col min="8" max="8" width="19.578125"/>
     <col min="9" max="9" width="39"/>
-    <col min="10" max="13" width="11.7109375"/>
-    <col min="14" max="1025" width="8.7109375"/>
+    <col min="10" max="13" width="11.68359375"/>
+    <col min="14" max="1025" width="8.68359375"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -7818,7 +7889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -7841,7 +7912,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -7867,7 +7938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -7893,7 +7964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -7919,7 +7990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -7942,7 +8013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -7965,7 +8036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -8000,7 +8071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -8029,7 +8100,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -8056,7 +8127,7 @@
       </c>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -8083,7 +8154,7 @@
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -8110,7 +8181,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -8139,7 +8210,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -8166,7 +8237,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="12.9" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Allineamento retail fase funzionante
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -1269,49 +1269,46 @@
     <t>Indicatore 53 - XRA_30GG_100_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Le possibili valorizzazioni del flag sono 0 oppure 1.
+    <t>Indicatore 200 - XRA_MEANMISS_SCONF_L3M</t>
+  </si>
+  <si>
+    <t>Media sul trimestre dell'importo di sconfino per cassa, calcolata considerando un valore pari a zero per le mensilità in cui è presente uno sconfino</t>
+  </si>
+  <si>
+    <t>Indicatore 150 - FLAG_SCONF_NON_AUTOR_1G</t>
+  </si>
+  <si>
+    <t>Indicatore 151 - FLAG_SCONF_NON_AUTOR_90G</t>
+  </si>
+  <si>
+    <t>Le possibili valorizzazioni del flag sono 0 oppure 1.
 Il flag sarà uguale a 1 in presenza di uno sconfino superiore a 30 giorni, di importo superiore a 100 euro e oltre la soglia di materialità del 2%. 
-In tutte le restanti casistiche il flag dovrà essere uguale a 0.
-In particolare, per il calcolo della soglia di materialità dovrà essere considerato il massimo tra: 
-- il rapporto fra sconfino per cassa e utilizzato per cassa e non, entrambi valutati alla data; 
-- il rapporto fra lo sconfino per cassa e utilizzato per cassa e non, entrambi valutati negli ultimi 90 giorni.  </t>
-  </si>
-  <si>
-    <t>Indicatore 200 - XRA_MEANMISS_SCONF_L3M</t>
-  </si>
-  <si>
-    <t>Media sul trimestre dell'importo di sconfino per cassa, calcolata considerando un valore pari a zero per le mensilità in cui è presente uno sconfino</t>
-  </si>
-  <si>
-    <t>Indicatore 150 - FLAG_SCONF_NON_AUTOR_1G</t>
-  </si>
-  <si>
-    <t>Indicatore 151 - FLAG_SCONF_NON_AUTOR_90G</t>
-  </si>
-  <si>
-    <t>l'indiatore è calcolato come il massimo tra il (FLG_SCONF_NON_AUTOR_1G; FLG_SCONF_MAX_NO_AUTOR_89GG)                                                                                                                                          Per ogni controparte sndg, viene indicata la presenza di sconfini autorizzati negli ultimi 90 giorni. L'indicatore assume valore:
-- 0, se il rmassimo valore assunto dall'indicatore 50 negli ultimi 90 giorni è 0;
-- 1, se il rmassimo valore assunto dall'indicatore 50 negli ultimi 90 giorni è 1;
-- missing, se l'indicatore 50 negli ultimi 90 giorni è sempre missing;</t>
-  </si>
-  <si>
-    <t>l'indicatore è calcolato come il rapporto tra l'importo complessivo degli sconfini "autorizzati" all'interno del flusso autor e l'importo di sconfino per cassa XRA                                                                                                                                              Per ogni controparte SNDG, l'indicatore verifica la presenza di sconfini autorizzati tra quello/quelli presenti nella giornata in oggetto di analisi. 
-Stabilita giornalmente la presenza di sconfini autorizzati, l'indicatore assume valore:
-- 0, se il rapporto tra lo sconfino complessivo giornaliero AUTOR e lo sconfino giornaliero XRA è maggiore o uguale a 1
-- 1, se il rapporto tra lo sconfino complessivo giornaliero AUTOR e lo sconfino giornaliero XRA è minore di 1
-- missing, se il rapporto tra lo sconfino complessivo giornaliero AUTOR e lo sconfino giornaliero XRA è missing</t>
+In tutte le restanti casistiche il flag dovrà essere uguale a 0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l'indicatore è calcolato come il rapporto tra l'importo complessivo degli sconfini "autorizzati" all'interno del flusso autor e l'importo di sconfino per cassa XRA                                                                                                                                              Per ogni controparte SNDG, l'indicatore verifica la presenza di sconfini autorizzati tra quello/quelli presenti nella giornata in oggetto di analisi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">l'indiatore è calcolato come il massimo tra il (FLG_SCONF_NON_AUTOR_1G; FLG_SCONF_MAX_NO_AUTOR_89GG)                                                                                                                                          Per ogni controparte sndg, viene indicata la </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1463,84 +1460,84 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1550,13 +1547,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1658,7 +1658,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1089062</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>813940</xdr:rowOff>
+      <xdr:rowOff>242440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1722,7 +1722,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1089062</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>813940</xdr:rowOff>
+      <xdr:rowOff>242440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1786,7 +1786,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1089062</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>813940</xdr:rowOff>
+      <xdr:rowOff>242440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1850,7 +1850,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1089062</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>813940</xdr:rowOff>
+      <xdr:rowOff>242440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1914,7 +1914,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1089062</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>813940</xdr:rowOff>
+      <xdr:rowOff>242440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD34"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2678,7 +2678,7 @@
     <col min="12" max="12" width="19.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="1019" width="8.7109375"/>
+    <col min="15" max="1017" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -4019,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>11</v>
       </c>
@@ -4029,8 +4029,8 @@
       <c r="C32" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="D32" s="32" t="s">
-        <v>398</v>
+      <c r="D32" s="33" t="s">
+        <v>402</v>
       </c>
       <c r="E32" s="32" t="s">
         <v>357</v>
@@ -4822,13 +4822,13 @@
         <v>383</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E50" s="32" t="s">
         <v>384</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G50" s="34">
         <v>249</v>
@@ -6626,13 +6626,13 @@
         <v>385</v>
       </c>
       <c r="D91" s="32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E91" s="32" t="s">
         <v>387</v>
       </c>
       <c r="F91" s="32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G91" s="34">
         <v>290</v>
@@ -6670,13 +6670,13 @@
         <v>386</v>
       </c>
       <c r="D92" s="32" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E92" s="32" t="s">
         <v>388</v>
       </c>
       <c r="F92" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G92" s="34">
         <v>291</v>
@@ -6727,8 +6727,8 @@
   <dimension ref="A1:F92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7260,7 +7260,7 @@
       <c r="E31" t="s">
         <v>339</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="37" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rimozione hide colums per gli indicatori
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -2658,8 +2658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="20" t="s">
         <v>45</v>
@@ -2989,7 +2989,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="20" t="s">
         <v>45</v>
@@ -3033,7 +3033,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>45</v>
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>45</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>45</v>
@@ -3164,7 +3164,7 @@
       <c r="H12" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="30" t="b">
+      <c r="I12" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J12" s="30" t="s">
@@ -3208,8 +3208,8 @@
       <c r="H13" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="30" t="b">
-        <v>1</v>
+      <c r="I13" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>45</v>
@@ -3252,8 +3252,8 @@
       <c r="H14" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="30" t="b">
-        <v>1</v>
+      <c r="I14" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>45</v>
@@ -3296,8 +3296,8 @@
       <c r="H15" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="30" t="b">
-        <v>1</v>
+      <c r="I15" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J15" s="30" t="s">
         <v>45</v>
@@ -3340,8 +3340,8 @@
       <c r="H16" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="30" t="b">
-        <v>1</v>
+      <c r="I16" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J16" s="30" t="s">
         <v>45</v>
@@ -3384,8 +3384,8 @@
       <c r="H17" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="30" t="b">
-        <v>1</v>
+      <c r="I17" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>45</v>
@@ -3428,8 +3428,8 @@
       <c r="H18" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="30" t="b">
-        <v>1</v>
+      <c r="I18" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J18" s="30" t="s">
         <v>45</v>
@@ -3472,8 +3472,8 @@
       <c r="H19" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="30" t="b">
-        <v>1</v>
+      <c r="I19" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J19" s="30" t="s">
         <v>45</v>
@@ -3516,8 +3516,8 @@
       <c r="H20" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="30" t="b">
-        <v>1</v>
+      <c r="I20" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J20" s="30" t="s">
         <v>45</v>
@@ -3560,8 +3560,8 @@
       <c r="H21" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="30" t="b">
-        <v>1</v>
+      <c r="I21" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J21" s="30" t="s">
         <v>45</v>
@@ -3604,8 +3604,8 @@
       <c r="H22" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="30" t="b">
-        <v>1</v>
+      <c r="I22" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>45</v>
@@ -3648,8 +3648,8 @@
       <c r="H23" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="30" t="b">
-        <v>1</v>
+      <c r="I23" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J23" s="30" t="s">
         <v>45</v>
@@ -3692,8 +3692,8 @@
       <c r="H24" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="30" t="b">
-        <v>1</v>
+      <c r="I24" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J24" s="30" t="s">
         <v>45</v>
@@ -3736,7 +3736,7 @@
       <c r="H25" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="30" t="b">
+      <c r="I25" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J25" s="30" t="s">
@@ -3780,8 +3780,8 @@
       <c r="H26" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="30" t="b">
-        <v>1</v>
+      <c r="I26" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J26" s="30" t="s">
         <v>45</v>
@@ -3824,8 +3824,8 @@
       <c r="H27" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="30" t="b">
-        <v>1</v>
+      <c r="I27" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J27" s="30" t="s">
         <v>45</v>
@@ -3868,8 +3868,8 @@
       <c r="H28" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="30" t="b">
-        <v>1</v>
+      <c r="I28" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>45</v>
@@ -3912,7 +3912,7 @@
       <c r="H29" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="30" t="b">
+      <c r="I29" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J29" s="30" t="s">
@@ -3956,7 +3956,7 @@
       <c r="H30" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="30" t="b">
+      <c r="I30" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J30" s="30" t="s">
@@ -4000,7 +4000,7 @@
       <c r="H31" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="30" t="b">
+      <c r="I31" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J31" s="30" t="s">
@@ -4044,8 +4044,8 @@
       <c r="H32" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="30" t="b">
-        <v>1</v>
+      <c r="I32" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J32" s="30" t="s">
         <v>45</v>
@@ -4089,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="20" t="s">
         <v>45</v>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" s="20" t="s">
         <v>45</v>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="20" t="s">
         <v>45</v>
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="20" t="s">
         <v>45</v>
@@ -4749,7 +4749,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>45</v>
@@ -4792,7 +4792,7 @@
       <c r="H49" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="30" t="b">
+      <c r="I49" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J49" s="30" t="s">
@@ -4836,7 +4836,7 @@
       <c r="H50" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I50" s="30" t="b">
+      <c r="I50" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J50" s="30" t="s">
@@ -4880,7 +4880,7 @@
       <c r="H51" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="30" t="b">
+      <c r="I51" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J51" s="30" t="s">
@@ -4924,7 +4924,7 @@
       <c r="H52" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I52" s="30" t="b">
+      <c r="I52" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J52" s="30" t="s">
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="I89" s="20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J89" s="20" t="s">
         <v>45</v>
@@ -6596,7 +6596,7 @@
       <c r="H90" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I90" s="30" t="b">
+      <c r="I90" s="20" t="b">
         <v>0</v>
       </c>
       <c r="J90" s="30" t="s">
@@ -6640,8 +6640,8 @@
       <c r="H91" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I91" s="30" t="b">
-        <v>1</v>
+      <c r="I91" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J91" s="30" t="s">
         <v>45</v>
@@ -6684,8 +6684,8 @@
       <c r="H92" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="I92" s="30" t="b">
-        <v>1</v>
+      <c r="I92" s="20" t="b">
+        <v>0</v>
       </c>
       <c r="J92" s="30" t="s">
         <v>45</v>
@@ -6726,7 +6726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>

</xml_diff>

<commit_message>
Aggiunti 104 e 900 alle librerie
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="436">
   <si>
     <t>Variable</t>
   </si>
@@ -1372,6 +1372,18 @@
   </si>
   <si>
     <t>L'indicatore assume il valore 1 se per la controparte oggetto di valutazione EW è riscontrata la presenza, presso altre banche, di garanzie rilasciate a favore di un nominativo a sofferenza o a procedura concorsuale, quando l’importo è significativo (l’anomalia è considerata significativa quando l’importo della sofferenza garantit</t>
+  </si>
+  <si>
+    <t>RETAIL_IND_900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dal flusso SISBA l'indicatore ricava e valorizza tutte le forme tecniche associate alla controparte. </t>
+  </si>
+  <si>
+    <t>IND_900</t>
+  </si>
+  <si>
+    <t>Indicatore 900 - Product mix</t>
   </si>
 </sst>
 </file>
@@ -2747,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7101,16 +7113,48 @@
       </c>
     </row>
     <row r="100" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="34"/>
-      <c r="B100" s="31"/>
-      <c r="G100" s="34"/>
-      <c r="H100" s="34"/>
-      <c r="I100" s="34"/>
-      <c r="J100" s="34"/>
-      <c r="K100" s="34"/>
-      <c r="L100" s="34"/>
-      <c r="M100" s="34"/>
-      <c r="N100" s="34"/>
+      <c r="A100" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="31" t="s">
+        <v>432</v>
+      </c>
+      <c r="C100" s="32" t="s">
+        <v>432</v>
+      </c>
+      <c r="D100" s="32" t="s">
+        <v>433</v>
+      </c>
+      <c r="E100" s="32" t="s">
+        <v>434</v>
+      </c>
+      <c r="F100" s="32" t="s">
+        <v>435</v>
+      </c>
+      <c r="G100" s="14">
+        <v>297</v>
+      </c>
+      <c r="H100" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J100" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="K100" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L100" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="M100" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="N100" s="21" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -7121,11 +7165,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8814,6 +8858,23 @@
         <v>386</v>
       </c>
       <c r="F99" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" t="s">
+        <v>432</v>
+      </c>
+      <c r="C100" t="s">
+        <v>432</v>
+      </c>
+      <c r="E100" t="s">
+        <v>432</v>
+      </c>
+      <c r="F100" s="17" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambio nome indicatori 107 110
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernando.monaco\Desktop\ISP\SorgentiGIT\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="26520" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -1032,9 +1032,6 @@
     <t>Indicatore 109 - Coefficiente rata arretrata per prodotti rateali con RID/MAV</t>
   </si>
   <si>
-    <t>Indicatore 110 - Numero di giorni di scaduto delle rate arretrate per prodotti rateali con RID/MAV</t>
-  </si>
-  <si>
     <t>Indicatore 111 - Importo delle rate arretrate per prodotti rateali con RID/MAV</t>
   </si>
   <si>
@@ -1331,9 +1328,6 @@
     <t>Indicatore 112 - Coefficiente rata arretrata per il prodotto "cessione del quinto"</t>
   </si>
   <si>
-    <t>Indicatore 113 - Numero di giorni di scaduto delle rate arretrate per il prodotto "cessione del quinto"</t>
-  </si>
-  <si>
     <t>RETAIL_IND_101</t>
   </si>
   <si>
@@ -1384,6 +1378,12 @@
   </si>
   <si>
     <t>Indicatore 900 - Product mix</t>
+  </si>
+  <si>
+    <t>Indicatore 113 - Giorni di scaduto delle rate arretrate per il prodotto "cessione del quinto"</t>
+  </si>
+  <si>
+    <t>Indicatore 110 - Giorni di scaduto delle rate arretrate per prodotti rateali con RID/MAV</t>
   </si>
 </sst>
 </file>
@@ -2759,30 +2759,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="B89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="15" customWidth="1"/>
     <col min="2" max="2" width="21" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.5546875" customWidth="1"/>
     <col min="7" max="7" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="1017" width="8.7109375"/>
+    <col min="8" max="8" width="21.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="1017" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2800,7 +2800,7 @@
       <c r="M1" s="13"/>
       <c r="N1" s="13"/>
     </row>
-    <row r="2" spans="1:14" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="8" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>11</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>11</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>11</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>11</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
         <v>11</v>
       </c>
@@ -3328,24 +3328,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G14" s="14">
         <v>211</v>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
         <v>11</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30" t="s">
         <v>11</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30" t="s">
         <v>11</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
         <v>11</v>
       </c>
@@ -3548,24 +3548,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="31" t="s">
+        <v>375</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="E19" s="32" t="s">
         <v>376</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="D19" s="32" t="s">
+      <c r="F19" s="32" t="s">
         <v>391</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>392</v>
       </c>
       <c r="G19" s="14">
         <v>216</v>
@@ -3592,24 +3592,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D20" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="F20" s="32" t="s">
         <v>393</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>378</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>394</v>
       </c>
       <c r="G20" s="14">
         <v>217</v>
@@ -3636,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
         <v>11</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
         <v>11</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>11</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
         <v>11</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
         <v>11</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>11</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
         <v>11</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>11</v>
       </c>
@@ -3988,24 +3988,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>204</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G29" s="14">
         <v>226</v>
@@ -4032,24 +4032,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>205</v>
       </c>
       <c r="E30" s="32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G30" s="14">
         <v>227</v>
@@ -4076,21 +4076,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>204</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F31" s="32" t="s">
         <v>220</v>
@@ -4120,24 +4120,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="32" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D32" s="33" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G32" s="14">
         <v>229</v>
@@ -4164,21 +4164,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D33" t="s">
         <v>206</v>
       </c>
       <c r="E33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F33" t="s">
         <v>221</v>
@@ -4208,21 +4208,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D34" t="s">
         <v>207</v>
       </c>
       <c r="E34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F34" t="s">
         <v>222</v>
@@ -4252,21 +4252,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D35" t="s">
         <v>208</v>
       </c>
       <c r="E35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F35" t="s">
         <v>223</v>
@@ -4296,21 +4296,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
         <v>209</v>
       </c>
       <c r="E36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F36" t="s">
         <v>224</v>
@@ -4340,21 +4340,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D37" t="s">
         <v>210</v>
       </c>
       <c r="E37" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F37" t="s">
         <v>225</v>
@@ -4384,21 +4384,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D38" t="s">
         <v>211</v>
       </c>
       <c r="E38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F38" t="s">
         <v>226</v>
@@ -4428,21 +4428,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D39" t="s">
         <v>212</v>
       </c>
       <c r="E39" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F39" t="s">
         <v>227</v>
@@ -4472,21 +4472,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D40" t="s">
         <v>213</v>
       </c>
       <c r="E40" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F40" t="s">
         <v>228</v>
@@ -4516,21 +4516,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D41" t="s">
         <v>214</v>
       </c>
       <c r="E41" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F41" t="s">
         <v>229</v>
@@ -4560,21 +4560,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D42" t="s">
         <v>215</v>
       </c>
       <c r="E42" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F42" t="s">
         <v>230</v>
@@ -4604,21 +4604,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D43" t="s">
         <v>216</v>
       </c>
       <c r="E43" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F43" t="s">
         <v>231</v>
@@ -4648,21 +4648,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D44" t="s">
         <v>217</v>
       </c>
       <c r="E44" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F44" t="s">
         <v>232</v>
@@ -4692,21 +4692,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D45" t="s">
         <v>218</v>
       </c>
       <c r="E45" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F45" t="s">
         <v>233</v>
@@ -4736,21 +4736,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D46" t="s">
         <v>219</v>
       </c>
       <c r="E46" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F46" t="s">
         <v>234</v>
@@ -4780,21 +4780,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F47" t="s">
         <v>235</v>
@@ -4824,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
         <v>11</v>
       </c>
@@ -4868,24 +4868,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D49" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E49" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F49" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G49" s="14">
         <v>246</v>
@@ -4912,24 +4912,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C50" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D50" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E50" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F50" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G50" s="14">
         <v>247</v>
@@ -4956,24 +4956,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D51" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E51" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F51" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G51" s="14">
         <v>248</v>
@@ -5000,24 +5000,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D52" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E52" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F52" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G52" s="14">
         <v>249</v>
@@ -5044,24 +5044,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D53" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E53" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F53" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G53" s="14">
         <v>250</v>
@@ -5088,7 +5088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="30" t="s">
         <v>11</v>
       </c>
@@ -5132,24 +5132,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="E55" s="32" t="s">
         <v>383</v>
       </c>
-      <c r="C55" s="32" t="s">
-        <v>383</v>
-      </c>
-      <c r="D55" s="32" t="s">
-        <v>399</v>
-      </c>
-      <c r="E55" s="32" t="s">
-        <v>384</v>
-      </c>
       <c r="F55" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G55" s="14">
         <v>252</v>
@@ -5176,7 +5176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="30" t="s">
         <v>11</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="30" t="s">
         <v>11</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
         <v>11</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
         <v>11</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
         <v>11</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
         <v>11</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
         <v>11</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
         <v>11</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
         <v>11</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
         <v>11</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
         <v>11</v>
       </c>
@@ -5660,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
         <v>11</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
         <v>11</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
         <v>11</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="20" t="s">
         <v>11</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="20" t="s">
         <v>11</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="20" t="s">
         <v>11</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="20" t="s">
         <v>11</v>
       </c>
@@ -5968,7 +5968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="20" t="s">
         <v>11</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="20" t="s">
         <v>11</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="20" t="s">
         <v>11</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="20" t="s">
         <v>11</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="20" t="s">
         <v>11</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="20" t="s">
         <v>11</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="20" t="s">
         <v>11</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="20" t="s">
         <v>11</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="20" t="s">
         <v>11</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="20" t="s">
         <v>11</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="20" t="s">
         <v>11</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="20" t="s">
         <v>11</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="29" t="s">
         <v>11</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="20" t="s">
         <v>11</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>302</v>
       </c>
       <c r="D87" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E87" t="s">
         <v>311</v>
@@ -6584,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="20" t="s">
         <v>11</v>
       </c>
@@ -6595,7 +6595,7 @@
         <v>303</v>
       </c>
       <c r="D88" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E88" t="s">
         <v>312</v>
@@ -6628,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="20" t="s">
         <v>11</v>
       </c>
@@ -6639,7 +6639,7 @@
         <v>304</v>
       </c>
       <c r="D89" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E89" t="s">
         <v>313</v>
@@ -6672,7 +6672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="20" t="s">
         <v>11</v>
       </c>
@@ -6683,7 +6683,7 @@
         <v>305</v>
       </c>
       <c r="D90" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E90" t="s">
         <v>314</v>
@@ -6716,7 +6716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="20" t="s">
         <v>11</v>
       </c>
@@ -6727,13 +6727,13 @@
         <v>306</v>
       </c>
       <c r="D91" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E91" t="s">
         <v>315</v>
       </c>
       <c r="F91" t="s">
-        <v>324</v>
+        <v>435</v>
       </c>
       <c r="G91" s="14">
         <v>288</v>
@@ -6760,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="20" t="s">
         <v>11</v>
       </c>
@@ -6771,13 +6771,13 @@
         <v>307</v>
       </c>
       <c r="D92" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E92" t="s">
         <v>316</v>
       </c>
       <c r="F92" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G92" s="14">
         <v>289</v>
@@ -6804,24 +6804,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C93" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D93" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E93" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F93" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G93" s="14">
         <v>290</v>
@@ -6848,24 +6848,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C94" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D94" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E94" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F94" t="s">
-        <v>418</v>
+        <v>434</v>
       </c>
       <c r="G94" s="14">
         <v>291</v>
@@ -6892,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="20" t="s">
         <v>11</v>
       </c>
@@ -6903,13 +6903,13 @@
         <v>308</v>
       </c>
       <c r="D95" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E95" t="s">
         <v>317</v>
       </c>
       <c r="F95" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G95" s="14">
         <v>292</v>
@@ -6936,7 +6936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="105" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96" s="20" t="s">
         <v>11</v>
       </c>
@@ -6947,13 +6947,13 @@
         <v>309</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E96" t="s">
         <v>318</v>
       </c>
       <c r="F96" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G96" s="14">
         <v>293</v>
@@ -6980,7 +6980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" s="32" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" s="32" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="30" t="s">
         <v>11</v>
       </c>
@@ -6991,13 +6991,13 @@
         <v>310</v>
       </c>
       <c r="D97" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E97" s="32" t="s">
         <v>319</v>
       </c>
       <c r="F97" s="32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G97" s="14">
         <v>294</v>
@@ -7024,24 +7024,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F98" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G98" s="14">
         <v>295</v>
@@ -7068,24 +7068,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D99" s="32" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F99" s="32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G99" s="14">
         <v>296</v>
@@ -7112,24 +7112,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B100" s="31" t="s">
+        <v>430</v>
+      </c>
+      <c r="C100" s="32" t="s">
+        <v>430</v>
+      </c>
+      <c r="D100" s="32" t="s">
+        <v>431</v>
+      </c>
+      <c r="E100" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="C100" s="32" t="s">
-        <v>432</v>
-      </c>
-      <c r="D100" s="32" t="s">
+      <c r="F100" s="32" t="s">
         <v>433</v>
-      </c>
-      <c r="E100" s="32" t="s">
-        <v>434</v>
-      </c>
-      <c r="F100" s="32" t="s">
-        <v>435</v>
       </c>
       <c r="G100" s="14">
         <v>297</v>
@@ -7167,22 +7167,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="48.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375"/>
+    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -7192,7 +7192,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="27"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -7399,24 +7399,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -7484,41 +7484,41 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7586,7 +7586,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -7603,7 +7603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -7654,330 +7654,330 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F31" s="36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F32" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E34" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F34" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E35" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E36" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F36" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F39" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F40" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E41" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F41" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F42" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E43" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F43" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F44" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F45" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E46" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F46" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F47" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -7994,92 +7994,92 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E49" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F49" s="37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C50" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E50" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F50" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E51" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F51" s="37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E52" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E53" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -8096,24 +8096,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C55" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E55" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F55" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -8232,7 +8232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -8334,7 +8334,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -8402,7 +8402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -8419,7 +8419,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -8470,7 +8470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -8538,7 +8538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -8572,7 +8572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -8623,7 +8623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -8657,7 +8657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -8691,7 +8691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -8725,7 +8725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -8742,41 +8742,41 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>11</v>
       </c>
       <c r="B93" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C93" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E93" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F93" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>11</v>
       </c>
       <c r="B94" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C94" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E94" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F94" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -8827,52 +8827,52 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>11</v>
       </c>
       <c r="B98" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C98" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E98" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F98" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E99" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F99" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>11</v>
       </c>
       <c r="B100" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C100" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E100" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F100" s="17" t="s">
         <v>23</v>
@@ -8894,19 +8894,19 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625"/>
-    <col min="2" max="3" width="19.5703125"/>
-    <col min="4" max="4" width="13.7109375"/>
-    <col min="5" max="7" width="11.7109375"/>
-    <col min="8" max="8" width="19.5703125"/>
+    <col min="1" max="1" width="27.33203125"/>
+    <col min="2" max="3" width="19.5546875"/>
+    <col min="4" max="4" width="13.6640625"/>
+    <col min="5" max="7" width="11.6640625"/>
+    <col min="8" max="8" width="19.5546875"/>
     <col min="9" max="9" width="39"/>
-    <col min="10" max="13" width="11.7109375"/>
-    <col min="14" max="1025" width="8.7109375"/>
+    <col min="10" max="13" width="11.6640625"/>
+    <col min="14" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -8964,7 +8964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -8990,7 +8990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -9065,7 +9065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -9088,7 +9088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -9123,7 +9123,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -9152,7 +9152,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -9179,7 +9179,7 @@
       </c>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -9206,7 +9206,7 @@
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -9233,7 +9233,7 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -9262,7 +9262,7 @@
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -9289,7 +9289,7 @@
       </c>
       <c r="K16"/>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
cambiato tipo degli indicatori 112 113
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView topLeftCell="E82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6833,18 +6833,18 @@
         <v>0</v>
       </c>
       <c r="J93" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K93" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L93" s="19" t="b">
+        <v>46</v>
+      </c>
+      <c r="K93" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L93" s="15" t="b">
         <v>0</v>
       </c>
       <c r="M93" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="N93" s="15" t="b">
+      <c r="N93" s="21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6877,18 +6877,18 @@
         <v>0</v>
       </c>
       <c r="J94" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K94" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L94" s="19" t="b">
+        <v>46</v>
+      </c>
+      <c r="K94" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L94" s="15" t="b">
         <v>0</v>
       </c>
       <c r="M94" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="N94" s="15" t="b">
+      <c r="N94" s="21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7168,8 +7168,8 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8755,8 +8755,8 @@
       <c r="E93" t="s">
         <v>424</v>
       </c>
-      <c r="F93" s="37" t="s">
-        <v>23</v>
+      <c r="F93" s="17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -8772,8 +8772,8 @@
       <c r="E94" t="s">
         <v>425</v>
       </c>
-      <c r="F94" s="37" t="s">
-        <v>23</v>
+      <c r="F94" s="17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
aggiornamento retail e bug fix 29
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/52_Inst_Variable_RETAIL.xlsx
@@ -1778,7 +1778,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1842,7 +1842,7 @@
         <xdr:cNvPr id="4" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1906,7 +1906,7 @@
         <xdr:cNvPr id="5" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1970,7 +1970,7 @@
         <xdr:cNvPr id="6" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2034,7 +2034,7 @@
         <xdr:cNvPr id="7" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2098,7 +2098,7 @@
         <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2152,7 +2152,7 @@
         <xdr:cNvPr id="13" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2216,7 +2216,7 @@
         <xdr:cNvPr id="14" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2280,7 +2280,7 @@
         <xdr:cNvPr id="15" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2344,7 +2344,7 @@
         <xdr:cNvPr id="16" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2408,7 +2408,7 @@
         <xdr:cNvPr id="17" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2472,7 +2472,7 @@
         <xdr:cNvPr id="3074" name="shapetype_202" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000020C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2771,8 +2771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="G45" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5078,25 +5078,25 @@
       <c r="G53" s="14">
         <v>250</v>
       </c>
-      <c r="H53" s="20" t="b">
+      <c r="H53" s="30" t="b">
         <v>0</v>
       </c>
       <c r="I53" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="J53" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="K53" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L53" s="19" t="b">
+      <c r="J53" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K53" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L53" s="34" t="b">
         <v>0</v>
       </c>
       <c r="M53" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="N53" s="15" t="b">
+      <c r="N53" s="21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7224,8 +7224,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50:A52"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8132,7 +8132,7 @@
         <v>421</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>